<commit_message>
A lot of bugs have been fixed
</commit_message>
<xml_diff>
--- a/sources/lab_111/tables/measures_1.xlsx
+++ b/sources/lab_111/tables/measures_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\LabaMaker\lab_111\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\LabaMaker\sources\lab_111\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630378DF-661F-4E44-A976-7AC6227200C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946A30A2-AC76-4D67-8220-D23845FD75A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>№</t>
   </si>
@@ -33,10 +33,7 @@
     <t>R</t>
   </si>
   <si>
-    <t>R оц.</t>
-  </si>
-  <si>
-    <t>N вит.</t>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -367,7 +364,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -377,10 +374,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
First release (with bugs) of all data without data
</commit_message>
<xml_diff>
--- a/sources/lab_111/tables/measures_1.xlsx
+++ b/sources/lab_111/tables/measures_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\LabaMaker\sources\lab_111\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946A30A2-AC76-4D67-8220-D23845FD75A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1534BA45-9B13-42A4-A776-803968008B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15384" yWindow="972" windowWidth="14256" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>№</t>
   </si>
   <si>
-    <t>R</t>
+    <t>N, unit</t>
   </si>
   <si>
-    <t>N</t>
+    <t>R, Om</t>
+  </si>
+  <si>
+    <t>R_ev, Om</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -374,13 +377,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>